<commit_message>
Fix: test with jest
</commit_message>
<xml_diff>
--- a/project/modules/handler/ts/test/test.xlsx
+++ b/project/modules/handler/ts/test/test.xlsx
@@ -14,18 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Nombre</t>
   </si>
   <si>
     <t>Edad</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>María</t>
   </si>
 </sst>
 </file>
@@ -402,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -413,22 +407,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>